<commit_message>
Actualiza base de datos
</commit_message>
<xml_diff>
--- a/_estadistica-descriptiva/basesdedatos/CabreraTorresKennethRoy.xlsx
+++ b/_estadistica-descriptiva/basesdedatos/CabreraTorresKennethRoy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t xml:space="preserve">Lugar</t>
   </si>
@@ -73,7 +73,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,11 +95,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -156,7 +151,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,7 +175,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -287,8 +282,23 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>6.261256</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>-75.576454</v>
+      </c>
       <c r="D5" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>43579</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.506944444444444</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>